<commit_message>
Completed SO fields additions
</commit_message>
<xml_diff>
--- a/template/So_Template.xlsx
+++ b/template/So_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jihbi\xampp\htdocs\synctronix\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D46142A-43E0-4B72-BC55-46CC44EBBD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE402F-76AC-4C01-89B9-E23B8EEBA94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9341FD95-CFC6-421C-9B6B-E00C8B5A4387}"/>
   </bookViews>
   <sheets>
     <sheet name="customermaster" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Company Code</t>
   </si>
@@ -65,6 +65,21 @@
   </si>
   <si>
     <t>Destination Name</t>
+  </si>
+  <si>
+    <t>Deliver To Name</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Order Load</t>
+  </si>
+  <si>
+    <t>Order Quantity</t>
   </si>
 </sst>
 </file>
@@ -427,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7AE52E-5E3F-4816-BCAD-C318F36103B6}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,9 +464,15 @@
     <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,6 +516,21 @@
         <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>